<commit_message>
ActorLevelTable ActorTranscendTable 액터 레벨업 및 초월 테이블 추가
</commit_message>
<xml_diff>
--- a/Excel/Actor.xlsx
+++ b/Excel/Actor.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696E53EC-C412-4655-85B1-237C61DE0651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB930D4D-A710-4A6B-ACEF-B793DD5B85FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94481F1D-1D61-4E23-90DD-352B3DAB9527}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{94481F1D-1D61-4E23-90DD-352B3DAB9527}"/>
   </bookViews>
   <sheets>
     <sheet name="ActorTable" sheetId="2" r:id="rId1"/>
     <sheet name="ActorInfoTable" sheetId="4" r:id="rId2"/>
+    <sheet name="ActorLevelTable" sheetId="5" r:id="rId3"/>
+    <sheet name="ActorTranscendTable" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="226">
   <si>
     <t>Portrait_AngelicWarrior</t>
   </si>
@@ -696,6 +698,24 @@
   </si>
   <si>
     <t>Tenebro</t>
+  </si>
+  <si>
+    <t>level|Int</t>
+  </si>
+  <si>
+    <t>accumulatedAtk|Int</t>
+  </si>
+  <si>
+    <t>requiredCount|Int</t>
+  </si>
+  <si>
+    <t>requiredAccumulatedCount|Int</t>
+  </si>
+  <si>
+    <t>requiredGold|Int</t>
+  </si>
+  <si>
+    <t>transcend|Int</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C0BC1-FCA1-449A-8610-F80C265CA071}">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3695,4 +3715,2832 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A219A9F8-1530-48C4-A2DD-8656FA2CD589}">
+  <dimension ref="A1:F121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>63</v>
+      </c>
+      <c r="F9">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>99</v>
+      </c>
+      <c r="F11">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>143</v>
+      </c>
+      <c r="F13">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>168</v>
+      </c>
+      <c r="F14">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>195</v>
+      </c>
+      <c r="F15">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>224</v>
+      </c>
+      <c r="F16">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>31</v>
+      </c>
+      <c r="E17">
+        <v>255</v>
+      </c>
+      <c r="F17">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>33</v>
+      </c>
+      <c r="E18">
+        <v>288</v>
+      </c>
+      <c r="F18">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <v>323</v>
+      </c>
+      <c r="F19">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>37</v>
+      </c>
+      <c r="E20">
+        <v>360</v>
+      </c>
+      <c r="F20">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>399</v>
+      </c>
+      <c r="F21">
+        <v>12700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>440</v>
+      </c>
+      <c r="F22">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>483</v>
+      </c>
+      <c r="F23">
+        <v>14100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>528</v>
+      </c>
+      <c r="F24">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>47</v>
+      </c>
+      <c r="E25">
+        <v>575</v>
+      </c>
+      <c r="F25">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>49</v>
+      </c>
+      <c r="E26">
+        <v>624</v>
+      </c>
+      <c r="F26">
+        <v>16200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>51</v>
+      </c>
+      <c r="E27">
+        <v>675</v>
+      </c>
+      <c r="F27">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>53</v>
+      </c>
+      <c r="E28">
+        <v>728</v>
+      </c>
+      <c r="F28">
+        <v>17600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>55</v>
+      </c>
+      <c r="E29">
+        <v>783</v>
+      </c>
+      <c r="F29">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>57</v>
+      </c>
+      <c r="E30">
+        <v>840</v>
+      </c>
+      <c r="F30">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>39</v>
+      </c>
+      <c r="D31">
+        <v>59</v>
+      </c>
+      <c r="E31">
+        <v>899</v>
+      </c>
+      <c r="F31">
+        <v>19700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>40</v>
+      </c>
+      <c r="D32">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>960</v>
+      </c>
+      <c r="F32">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>63</v>
+      </c>
+      <c r="E33">
+        <v>1023</v>
+      </c>
+      <c r="F33">
+        <v>21100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>65</v>
+      </c>
+      <c r="E34">
+        <v>1088</v>
+      </c>
+      <c r="F34">
+        <v>21800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>43</v>
+      </c>
+      <c r="D35">
+        <v>67</v>
+      </c>
+      <c r="E35">
+        <v>1155</v>
+      </c>
+      <c r="F35">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>44</v>
+      </c>
+      <c r="D36">
+        <v>69</v>
+      </c>
+      <c r="E36">
+        <v>1224</v>
+      </c>
+      <c r="F36">
+        <v>23200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>45</v>
+      </c>
+      <c r="D37">
+        <v>71</v>
+      </c>
+      <c r="E37">
+        <v>1295</v>
+      </c>
+      <c r="F37">
+        <v>23900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>46</v>
+      </c>
+      <c r="D38">
+        <v>73</v>
+      </c>
+      <c r="E38">
+        <v>1368</v>
+      </c>
+      <c r="F38">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>47</v>
+      </c>
+      <c r="D39">
+        <v>75</v>
+      </c>
+      <c r="E39">
+        <v>1443</v>
+      </c>
+      <c r="F39">
+        <v>25300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>48</v>
+      </c>
+      <c r="D40">
+        <v>77</v>
+      </c>
+      <c r="E40">
+        <v>1520</v>
+      </c>
+      <c r="F40">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>49</v>
+      </c>
+      <c r="D41">
+        <v>79</v>
+      </c>
+      <c r="E41">
+        <v>1599</v>
+      </c>
+      <c r="F41">
+        <v>26700</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>30</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>31</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>32</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>33</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>34</v>
+      </c>
+      <c r="D46">
+        <v>9</v>
+      </c>
+      <c r="E46">
+        <v>24</v>
+      </c>
+      <c r="F46">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>35</v>
+      </c>
+      <c r="D47">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>35</v>
+      </c>
+      <c r="F47">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>13</v>
+      </c>
+      <c r="E48">
+        <v>48</v>
+      </c>
+      <c r="F48">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>37</v>
+      </c>
+      <c r="D49">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>63</v>
+      </c>
+      <c r="F49">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>38</v>
+      </c>
+      <c r="D50">
+        <v>17</v>
+      </c>
+      <c r="E50">
+        <v>80</v>
+      </c>
+      <c r="F50">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>39</v>
+      </c>
+      <c r="D51">
+        <v>19</v>
+      </c>
+      <c r="E51">
+        <v>99</v>
+      </c>
+      <c r="F51">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>40</v>
+      </c>
+      <c r="D52">
+        <v>21</v>
+      </c>
+      <c r="E52">
+        <v>120</v>
+      </c>
+      <c r="F52">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>41</v>
+      </c>
+      <c r="D53">
+        <v>23</v>
+      </c>
+      <c r="E53">
+        <v>143</v>
+      </c>
+      <c r="F53">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>42</v>
+      </c>
+      <c r="D54">
+        <v>25</v>
+      </c>
+      <c r="E54">
+        <v>168</v>
+      </c>
+      <c r="F54">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>43</v>
+      </c>
+      <c r="D55">
+        <v>27</v>
+      </c>
+      <c r="E55">
+        <v>195</v>
+      </c>
+      <c r="F55">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>44</v>
+      </c>
+      <c r="D56">
+        <v>29</v>
+      </c>
+      <c r="E56">
+        <v>224</v>
+      </c>
+      <c r="F56">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>16</v>
+      </c>
+      <c r="C57">
+        <v>45</v>
+      </c>
+      <c r="D57">
+        <v>31</v>
+      </c>
+      <c r="E57">
+        <v>255</v>
+      </c>
+      <c r="F57">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>17</v>
+      </c>
+      <c r="C58">
+        <v>46</v>
+      </c>
+      <c r="D58">
+        <v>33</v>
+      </c>
+      <c r="E58">
+        <v>288</v>
+      </c>
+      <c r="F58">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <v>47</v>
+      </c>
+      <c r="D59">
+        <v>35</v>
+      </c>
+      <c r="E59">
+        <v>323</v>
+      </c>
+      <c r="F59">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>19</v>
+      </c>
+      <c r="C60">
+        <v>48</v>
+      </c>
+      <c r="D60">
+        <v>37</v>
+      </c>
+      <c r="E60">
+        <v>360</v>
+      </c>
+      <c r="F60">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>49</v>
+      </c>
+      <c r="D61">
+        <v>39</v>
+      </c>
+      <c r="E61">
+        <v>399</v>
+      </c>
+      <c r="F61">
+        <v>12700</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>21</v>
+      </c>
+      <c r="C62">
+        <v>50</v>
+      </c>
+      <c r="D62">
+        <v>41</v>
+      </c>
+      <c r="E62">
+        <v>440</v>
+      </c>
+      <c r="F62">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>22</v>
+      </c>
+      <c r="C63">
+        <v>51</v>
+      </c>
+      <c r="D63">
+        <v>43</v>
+      </c>
+      <c r="E63">
+        <v>483</v>
+      </c>
+      <c r="F63">
+        <v>14100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>23</v>
+      </c>
+      <c r="C64">
+        <v>52</v>
+      </c>
+      <c r="D64">
+        <v>45</v>
+      </c>
+      <c r="E64">
+        <v>528</v>
+      </c>
+      <c r="F64">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>24</v>
+      </c>
+      <c r="C65">
+        <v>53</v>
+      </c>
+      <c r="D65">
+        <v>47</v>
+      </c>
+      <c r="E65">
+        <v>575</v>
+      </c>
+      <c r="F65">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>54</v>
+      </c>
+      <c r="D66">
+        <v>49</v>
+      </c>
+      <c r="E66">
+        <v>624</v>
+      </c>
+      <c r="F66">
+        <v>16200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>26</v>
+      </c>
+      <c r="C67">
+        <v>55</v>
+      </c>
+      <c r="D67">
+        <v>51</v>
+      </c>
+      <c r="E67">
+        <v>675</v>
+      </c>
+      <c r="F67">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>56</v>
+      </c>
+      <c r="D68">
+        <v>53</v>
+      </c>
+      <c r="E68">
+        <v>728</v>
+      </c>
+      <c r="F68">
+        <v>17600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>28</v>
+      </c>
+      <c r="C69">
+        <v>57</v>
+      </c>
+      <c r="D69">
+        <v>55</v>
+      </c>
+      <c r="E69">
+        <v>783</v>
+      </c>
+      <c r="F69">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>29</v>
+      </c>
+      <c r="C70">
+        <v>58</v>
+      </c>
+      <c r="D70">
+        <v>57</v>
+      </c>
+      <c r="E70">
+        <v>840</v>
+      </c>
+      <c r="F70">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>30</v>
+      </c>
+      <c r="C71">
+        <v>59</v>
+      </c>
+      <c r="D71">
+        <v>59</v>
+      </c>
+      <c r="E71">
+        <v>899</v>
+      </c>
+      <c r="F71">
+        <v>19700</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>31</v>
+      </c>
+      <c r="C72">
+        <v>60</v>
+      </c>
+      <c r="D72">
+        <v>61</v>
+      </c>
+      <c r="E72">
+        <v>960</v>
+      </c>
+      <c r="F72">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>32</v>
+      </c>
+      <c r="C73">
+        <v>61</v>
+      </c>
+      <c r="D73">
+        <v>63</v>
+      </c>
+      <c r="E73">
+        <v>1023</v>
+      </c>
+      <c r="F73">
+        <v>21100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>33</v>
+      </c>
+      <c r="C74">
+        <v>62</v>
+      </c>
+      <c r="D74">
+        <v>65</v>
+      </c>
+      <c r="E74">
+        <v>1088</v>
+      </c>
+      <c r="F74">
+        <v>21800</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>34</v>
+      </c>
+      <c r="C75">
+        <v>63</v>
+      </c>
+      <c r="D75">
+        <v>67</v>
+      </c>
+      <c r="E75">
+        <v>1155</v>
+      </c>
+      <c r="F75">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>35</v>
+      </c>
+      <c r="C76">
+        <v>64</v>
+      </c>
+      <c r="D76">
+        <v>69</v>
+      </c>
+      <c r="E76">
+        <v>1224</v>
+      </c>
+      <c r="F76">
+        <v>23200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>36</v>
+      </c>
+      <c r="C77">
+        <v>65</v>
+      </c>
+      <c r="D77">
+        <v>71</v>
+      </c>
+      <c r="E77">
+        <v>1295</v>
+      </c>
+      <c r="F77">
+        <v>23900</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>37</v>
+      </c>
+      <c r="C78">
+        <v>66</v>
+      </c>
+      <c r="D78">
+        <v>73</v>
+      </c>
+      <c r="E78">
+        <v>1368</v>
+      </c>
+      <c r="F78">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>38</v>
+      </c>
+      <c r="C79">
+        <v>67</v>
+      </c>
+      <c r="D79">
+        <v>75</v>
+      </c>
+      <c r="E79">
+        <v>1443</v>
+      </c>
+      <c r="F79">
+        <v>25300</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>39</v>
+      </c>
+      <c r="C80">
+        <v>68</v>
+      </c>
+      <c r="D80">
+        <v>77</v>
+      </c>
+      <c r="E80">
+        <v>1520</v>
+      </c>
+      <c r="F80">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>40</v>
+      </c>
+      <c r="C81">
+        <v>69</v>
+      </c>
+      <c r="D81">
+        <v>79</v>
+      </c>
+      <c r="E81">
+        <v>1599</v>
+      </c>
+      <c r="F81">
+        <v>26700</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>100</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <v>101</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83">
+        <v>3</v>
+      </c>
+      <c r="F83">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84">
+        <v>102</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
+      <c r="E84">
+        <v>8</v>
+      </c>
+      <c r="F84">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>103</v>
+      </c>
+      <c r="D85">
+        <v>7</v>
+      </c>
+      <c r="E85">
+        <v>15</v>
+      </c>
+      <c r="F85">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>104</v>
+      </c>
+      <c r="D86">
+        <v>9</v>
+      </c>
+      <c r="E86">
+        <v>24</v>
+      </c>
+      <c r="F86">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2</v>
+      </c>
+      <c r="B87">
+        <v>6</v>
+      </c>
+      <c r="C87">
+        <v>105</v>
+      </c>
+      <c r="D87">
+        <v>11</v>
+      </c>
+      <c r="E87">
+        <v>35</v>
+      </c>
+      <c r="F87">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+      <c r="C88">
+        <v>106</v>
+      </c>
+      <c r="D88">
+        <v>13</v>
+      </c>
+      <c r="E88">
+        <v>48</v>
+      </c>
+      <c r="F88">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <v>8</v>
+      </c>
+      <c r="C89">
+        <v>107</v>
+      </c>
+      <c r="D89">
+        <v>15</v>
+      </c>
+      <c r="E89">
+        <v>63</v>
+      </c>
+      <c r="F89">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>9</v>
+      </c>
+      <c r="C90">
+        <v>108</v>
+      </c>
+      <c r="D90">
+        <v>17</v>
+      </c>
+      <c r="E90">
+        <v>80</v>
+      </c>
+      <c r="F90">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>109</v>
+      </c>
+      <c r="D91">
+        <v>19</v>
+      </c>
+      <c r="E91">
+        <v>99</v>
+      </c>
+      <c r="F91">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2</v>
+      </c>
+      <c r="B92">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>110</v>
+      </c>
+      <c r="D92">
+        <v>21</v>
+      </c>
+      <c r="E92">
+        <v>120</v>
+      </c>
+      <c r="F92">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93">
+        <v>12</v>
+      </c>
+      <c r="C93">
+        <v>111</v>
+      </c>
+      <c r="D93">
+        <v>23</v>
+      </c>
+      <c r="E93">
+        <v>143</v>
+      </c>
+      <c r="F93">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94">
+        <v>112</v>
+      </c>
+      <c r="D94">
+        <v>25</v>
+      </c>
+      <c r="E94">
+        <v>168</v>
+      </c>
+      <c r="F94">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95">
+        <v>14</v>
+      </c>
+      <c r="C95">
+        <v>113</v>
+      </c>
+      <c r="D95">
+        <v>27</v>
+      </c>
+      <c r="E95">
+        <v>195</v>
+      </c>
+      <c r="F95">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+      <c r="C96">
+        <v>114</v>
+      </c>
+      <c r="D96">
+        <v>29</v>
+      </c>
+      <c r="E96">
+        <v>224</v>
+      </c>
+      <c r="F96">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>16</v>
+      </c>
+      <c r="C97">
+        <v>115</v>
+      </c>
+      <c r="D97">
+        <v>31</v>
+      </c>
+      <c r="E97">
+        <v>255</v>
+      </c>
+      <c r="F97">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>17</v>
+      </c>
+      <c r="C98">
+        <v>116</v>
+      </c>
+      <c r="D98">
+        <v>33</v>
+      </c>
+      <c r="E98">
+        <v>288</v>
+      </c>
+      <c r="F98">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>18</v>
+      </c>
+      <c r="C99">
+        <v>117</v>
+      </c>
+      <c r="D99">
+        <v>35</v>
+      </c>
+      <c r="E99">
+        <v>323</v>
+      </c>
+      <c r="F99">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>19</v>
+      </c>
+      <c r="C100">
+        <v>118</v>
+      </c>
+      <c r="D100">
+        <v>37</v>
+      </c>
+      <c r="E100">
+        <v>360</v>
+      </c>
+      <c r="F100">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>20</v>
+      </c>
+      <c r="C101">
+        <v>119</v>
+      </c>
+      <c r="D101">
+        <v>39</v>
+      </c>
+      <c r="E101">
+        <v>399</v>
+      </c>
+      <c r="F101">
+        <v>12700</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>21</v>
+      </c>
+      <c r="C102">
+        <v>120</v>
+      </c>
+      <c r="D102">
+        <v>41</v>
+      </c>
+      <c r="E102">
+        <v>440</v>
+      </c>
+      <c r="F102">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>2</v>
+      </c>
+      <c r="B103">
+        <v>22</v>
+      </c>
+      <c r="C103">
+        <v>121</v>
+      </c>
+      <c r="D103">
+        <v>43</v>
+      </c>
+      <c r="E103">
+        <v>483</v>
+      </c>
+      <c r="F103">
+        <v>14100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>2</v>
+      </c>
+      <c r="B104">
+        <v>23</v>
+      </c>
+      <c r="C104">
+        <v>122</v>
+      </c>
+      <c r="D104">
+        <v>45</v>
+      </c>
+      <c r="E104">
+        <v>528</v>
+      </c>
+      <c r="F104">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>2</v>
+      </c>
+      <c r="B105">
+        <v>24</v>
+      </c>
+      <c r="C105">
+        <v>123</v>
+      </c>
+      <c r="D105">
+        <v>47</v>
+      </c>
+      <c r="E105">
+        <v>575</v>
+      </c>
+      <c r="F105">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>25</v>
+      </c>
+      <c r="C106">
+        <v>124</v>
+      </c>
+      <c r="D106">
+        <v>49</v>
+      </c>
+      <c r="E106">
+        <v>624</v>
+      </c>
+      <c r="F106">
+        <v>16200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>26</v>
+      </c>
+      <c r="C107">
+        <v>125</v>
+      </c>
+      <c r="D107">
+        <v>51</v>
+      </c>
+      <c r="E107">
+        <v>675</v>
+      </c>
+      <c r="F107">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <v>27</v>
+      </c>
+      <c r="C108">
+        <v>126</v>
+      </c>
+      <c r="D108">
+        <v>53</v>
+      </c>
+      <c r="E108">
+        <v>728</v>
+      </c>
+      <c r="F108">
+        <v>17600</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>2</v>
+      </c>
+      <c r="B109">
+        <v>28</v>
+      </c>
+      <c r="C109">
+        <v>127</v>
+      </c>
+      <c r="D109">
+        <v>55</v>
+      </c>
+      <c r="E109">
+        <v>783</v>
+      </c>
+      <c r="F109">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>2</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110">
+        <v>128</v>
+      </c>
+      <c r="D110">
+        <v>57</v>
+      </c>
+      <c r="E110">
+        <v>840</v>
+      </c>
+      <c r="F110">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>2</v>
+      </c>
+      <c r="B111">
+        <v>30</v>
+      </c>
+      <c r="C111">
+        <v>129</v>
+      </c>
+      <c r="D111">
+        <v>59</v>
+      </c>
+      <c r="E111">
+        <v>899</v>
+      </c>
+      <c r="F111">
+        <v>19700</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>2</v>
+      </c>
+      <c r="B112">
+        <v>31</v>
+      </c>
+      <c r="C112">
+        <v>130</v>
+      </c>
+      <c r="D112">
+        <v>61</v>
+      </c>
+      <c r="E112">
+        <v>960</v>
+      </c>
+      <c r="F112">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>2</v>
+      </c>
+      <c r="B113">
+        <v>32</v>
+      </c>
+      <c r="C113">
+        <v>131</v>
+      </c>
+      <c r="D113">
+        <v>63</v>
+      </c>
+      <c r="E113">
+        <v>1023</v>
+      </c>
+      <c r="F113">
+        <v>21100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>33</v>
+      </c>
+      <c r="C114">
+        <v>132</v>
+      </c>
+      <c r="D114">
+        <v>65</v>
+      </c>
+      <c r="E114">
+        <v>1088</v>
+      </c>
+      <c r="F114">
+        <v>21800</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>2</v>
+      </c>
+      <c r="B115">
+        <v>34</v>
+      </c>
+      <c r="C115">
+        <v>133</v>
+      </c>
+      <c r="D115">
+        <v>67</v>
+      </c>
+      <c r="E115">
+        <v>1155</v>
+      </c>
+      <c r="F115">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116">
+        <v>35</v>
+      </c>
+      <c r="C116">
+        <v>134</v>
+      </c>
+      <c r="D116">
+        <v>69</v>
+      </c>
+      <c r="E116">
+        <v>1224</v>
+      </c>
+      <c r="F116">
+        <v>23200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117">
+        <v>36</v>
+      </c>
+      <c r="C117">
+        <v>135</v>
+      </c>
+      <c r="D117">
+        <v>71</v>
+      </c>
+      <c r="E117">
+        <v>1295</v>
+      </c>
+      <c r="F117">
+        <v>23900</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>2</v>
+      </c>
+      <c r="B118">
+        <v>37</v>
+      </c>
+      <c r="C118">
+        <v>136</v>
+      </c>
+      <c r="D118">
+        <v>73</v>
+      </c>
+      <c r="E118">
+        <v>1368</v>
+      </c>
+      <c r="F118">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <v>38</v>
+      </c>
+      <c r="C119">
+        <v>137</v>
+      </c>
+      <c r="D119">
+        <v>75</v>
+      </c>
+      <c r="E119">
+        <v>1443</v>
+      </c>
+      <c r="F119">
+        <v>25300</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120">
+        <v>39</v>
+      </c>
+      <c r="C120">
+        <v>138</v>
+      </c>
+      <c r="D120">
+        <v>77</v>
+      </c>
+      <c r="E120">
+        <v>1520</v>
+      </c>
+      <c r="F120">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121">
+        <v>40</v>
+      </c>
+      <c r="C121">
+        <v>139</v>
+      </c>
+      <c r="D121">
+        <v>79</v>
+      </c>
+      <c r="E121">
+        <v>1599</v>
+      </c>
+      <c r="F121">
+        <v>26700</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B90BAD2-7FC3-4CAF-BDC4-78BBB07EEBB6}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>600</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>800</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1000</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>2000</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>2500</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>2900</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>